<commit_message>
1st working version (with issues)
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Task</t>
   </si>
@@ -22,16 +22,25 @@
     <t>Estimate</t>
   </si>
   <si>
-    <t>Sort out relationship between render command and surface format</t>
-  </si>
-  <si>
-    <t>Get lights in engine and into shader</t>
-  </si>
-  <si>
     <t>Vertex welding in model compiler</t>
   </si>
   <si>
     <t>Textured surfaces</t>
+  </si>
+  <si>
+    <t>Refactoring - we need consistency across the board</t>
+  </si>
+  <si>
+    <t>Error handling - go on a robustness run, set standards for future work</t>
+  </si>
+  <si>
+    <t>Make it spin</t>
+  </si>
+  <si>
+    <t>Data drive lighting</t>
+  </si>
+  <si>
+    <t>Fix sorting issues</t>
   </si>
 </sst>
 </file>
@@ -379,10 +388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -400,15 +409,15 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="B3">
         <v>3</v>
@@ -416,18 +425,42 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B4">
-        <v>6</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B5">
+      <c r="B7">
         <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added depth stencil to fix z-sorting issues.
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Task</t>
   </si>
@@ -35,9 +35,6 @@
   </si>
   <si>
     <t>Data drive lighting</t>
-  </si>
-  <si>
-    <t>Fix sorting issues (use depth stencil gubbins)</t>
   </si>
 </sst>
 </file>
@@ -385,10 +382,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -406,31 +403,31 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B2">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B3">
-        <v>3</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B4">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5">
         <v>21</v>
@@ -438,17 +435,9 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B6">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7">
         <v>35</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Now exporting smoothed normals.
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Task</t>
   </si>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t>Data drive lighting</t>
+  </si>
+  <si>
+    <t>Fix normals problem on cylinder</t>
   </si>
 </sst>
 </file>
@@ -78,9 +81,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -382,10 +386,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="B2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -402,32 +406,32 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B2">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B3">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5">
         <v>21</v>
@@ -435,9 +439,17 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>3</v>
       </c>
-      <c r="B6">
+      <c r="B7">
         <v>35</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed bug in normals export.
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Task</t>
   </si>
@@ -35,9 +35,6 @@
   </si>
   <si>
     <t>Data drive lighting</t>
-  </si>
-  <si>
-    <t>Fix normals problem on cylinder</t>
   </si>
 </sst>
 </file>
@@ -81,10 +78,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -386,10 +382,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="A2:B2"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -406,51 +402,43 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="2">
-        <v>3</v>
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2">
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B3">
-        <v>4</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B4">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>21</v>
+        <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B6">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7">
-        <v>35</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Lighting is now driven my engine client. Fixed bug in untextured shader. Model to view is now an argument to the model viewer.
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -34,9 +34,6 @@
     <t>Error handling - go on a robustness run, set standards for future work</t>
   </si>
   <si>
-    <t>Data drive lighting</t>
-  </si>
-  <si>
     <t>Make exporter a GUP.  Build UI &amp; hook data into the max files</t>
   </si>
   <si>
@@ -44,6 +41,9 @@
   </si>
   <si>
     <t>Complete the Rorn Maths library</t>
+  </si>
+  <si>
+    <t>Make the path from Max-&gt;Model Viewer seamless</t>
   </si>
 </sst>
 </file>
@@ -394,7 +394,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -415,20 +415,20 @@
         <v>6</v>
       </c>
       <c r="B2">
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B3">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B4">
         <v>14</v>
@@ -468,7 +468,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9">
         <v>35</v>

</xml_diff>

<commit_message>
Updated error handling task.
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -31,9 +31,6 @@
     <t>Refactoring - we need consistency across the board</t>
   </si>
   <si>
-    <t>Error handling - go on a robustness run, set standards for future work</t>
-  </si>
-  <si>
     <t>Make exporter a GUP.  Build UI &amp; hook data into the max files</t>
   </si>
   <si>
@@ -44,6 +41,9 @@
   </si>
   <si>
     <t>Make the path from Max-&gt;Model Viewer seamless</t>
+  </si>
+  <si>
+    <t>Error handling - go on a robustness run, set standards for future work.  Ensure anythign that can go wrong is handled.</t>
   </si>
 </sst>
 </file>
@@ -394,12 +394,12 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="61.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="106.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -412,7 +412,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2">
         <v>14</v>
@@ -420,7 +420,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3">
         <v>4</v>
@@ -428,23 +428,23 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B4">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B5">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6">
         <v>21</v>
@@ -468,7 +468,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>35</v>

</xml_diff>

<commit_message>
Added some new tasks.
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Task</t>
   </si>
@@ -44,6 +44,12 @@
   </si>
   <si>
     <t>Error handling - go on a robustness run, set standards for future work.  Ensure anythign that can go wrong is handled.</t>
+  </si>
+  <si>
+    <t>Add full screen support</t>
+  </si>
+  <si>
+    <t>Add camera controls to model viewer</t>
   </si>
 </sst>
 </file>
@@ -391,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -452,25 +458,41 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7">
         <v>3</v>
-      </c>
-      <c r="B7">
-        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="B8">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>7</v>
       </c>
-      <c r="B9">
+      <c r="B11">
         <v>35</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added first raft of diagnostics.
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Task</t>
   </si>
@@ -47,9 +47,6 @@
   </si>
   <si>
     <t>Add camera controls to model viewer</t>
-  </si>
-  <si>
-    <t>Add logging mechanism. Find out why it's slow on the laptop.</t>
   </si>
   <si>
     <t>Error handling - go on a robustness run, set standards for future work.  Ensure anything that can go wrong is handled.</t>
@@ -400,10 +397,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -424,12 +421,12 @@
         <v>11</v>
       </c>
       <c r="B2">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="B3">
         <v>21</v>
@@ -437,15 +434,15 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B4">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5">
         <v>14</v>
@@ -453,57 +450,49 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="B6">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B7">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B8">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="B9">
-        <v>5</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B10">
-        <v>35</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B11">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>7</v>
-      </c>
-      <c r="B12">
         <v>35</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Implemented the renderer in terms of the Rorn maths library.
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -31,9 +31,6 @@
     <t>Make exporter a GUP.  Build UI &amp; hook data into the max files</t>
   </si>
   <si>
-    <t>Replace XNAMATH with a Rorn maths library</t>
-  </si>
-  <si>
     <t>Complete the Rorn Maths library</t>
   </si>
   <si>
@@ -47,6 +44,9 @@
   </si>
   <si>
     <t>Refactoring - we need consistency across the board - All 3 apps</t>
+  </si>
+  <si>
+    <t>Revise, understand and document the view and projection matrix builds</t>
   </si>
 </sst>
 </file>
@@ -397,7 +397,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -415,26 +415,26 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B2">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B3">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
         <v>4</v>
-      </c>
-      <c r="B4">
-        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -442,7 +442,7 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -450,39 +450,39 @@
         <v>8</v>
       </c>
       <c r="B6">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B7">
-        <v>5</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B8">
-        <v>35</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B9">
-        <v>14</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B10">
-        <v>35</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated todo list Deleted out of date model
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -14,15 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Task</t>
   </si>
   <si>
     <t>Estimate</t>
-  </si>
-  <si>
-    <t>Vertex welding in model compiler</t>
   </si>
   <si>
     <t>Textured surfaces</t>
@@ -397,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -418,7 +415,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2">
         <v>21</v>
@@ -426,7 +423,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3">
         <v>14</v>
@@ -434,7 +431,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B4">
         <v>4</v>
@@ -442,7 +439,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B5">
         <v>3</v>
@@ -450,7 +447,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6">
         <v>5</v>
@@ -458,7 +455,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B7">
         <v>35</v>
@@ -466,7 +463,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8">
         <v>7</v>
@@ -474,25 +471,17 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B9">
-        <v>14</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B10">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Phong exponent to export process.
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Task</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t>Error handling strategy in Model Compiler</t>
+  </si>
+  <si>
+    <t>Specular lighting</t>
   </si>
 </sst>
 </file>
@@ -90,9 +93,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -394,10 +398,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -414,74 +418,82 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2">
-        <v>21</v>
+      <c r="A2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="2">
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="B3">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B4">
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B5">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B6">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B7">
-        <v>35</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="B8">
-        <v>7</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="B9">
-        <v>35</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="B10">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>9</v>
       </c>
-      <c r="B10">
+      <c r="B11">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Specular lighting now working (I think) on untextured surfaces.
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Task</t>
   </si>
@@ -47,9 +47,6 @@
   </si>
   <si>
     <t>Error handling strategy in Model Compiler</t>
-  </si>
-  <si>
-    <t>Specular lighting</t>
   </si>
 </sst>
 </file>
@@ -93,10 +90,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -398,10 +394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -418,82 +414,74 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="2">
-        <v>4</v>
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B2">
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B3">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B4">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B6">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B7">
-        <v>5</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B8">
-        <v>35</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="B9">
-        <v>7</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B10">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Model data now uses 4D vectors.
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -19,7 +19,7 @@
     <author>Jonny</author>
   </authors>
   <commentList>
-    <comment ref="A8" authorId="0">
+    <comment ref="A7" authorId="0">
       <text>
         <r>
           <rPr>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Task</t>
   </si>
@@ -93,9 +93,6 @@
   </si>
   <si>
     <t>Spot lights within model</t>
-  </si>
-  <si>
-    <t>Move to 4D vectors in final model data</t>
   </si>
 </sst>
 </file>
@@ -152,10 +149,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -457,10 +453,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -477,48 +473,48 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="2">
-        <v>1</v>
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B3">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B4">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B5">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="B6">
-        <v>4</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B7">
         <v>21</v>
@@ -526,65 +522,57 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B8">
-        <v>21</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="B9">
-        <v>35</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B10">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="B11">
-        <v>3</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B12">
-        <v>70</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B13">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B14">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Model compiler can now compile textured materials (including textures themselves).
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -456,7 +456,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -477,7 +477,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Textured surfaces seem to be working well.  Test case was a TurboSquid pool table.
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -19,7 +19,7 @@
     <author>Jonny</author>
   </authors>
   <commentList>
-    <comment ref="A7" authorId="0">
+    <comment ref="A6" authorId="0">
       <text>
         <r>
           <rPr>
@@ -48,15 +48,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>Task</t>
   </si>
   <si>
     <t>Estimate</t>
-  </si>
-  <si>
-    <t>Textured surfaces</t>
   </si>
   <si>
     <t>Make exporter a GUP.  Build UI &amp; hook data into the max files</t>
@@ -453,10 +450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -474,39 +471,39 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B2">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="B5">
-        <v>4</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <v>21</v>
@@ -514,42 +511,42 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B7">
-        <v>21</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="B8">
-        <v>35</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B9">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="B10">
-        <v>3</v>
+        <v>70</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B11">
-        <v>70</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -557,7 +554,7 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -565,14 +562,6 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>14</v>
-      </c>
-      <c r="B14">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added better lighting for pool table. Updated todo list.
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -19,7 +19,55 @@
     <author>Jonny</author>
   </authors>
   <commentList>
-    <comment ref="A6" authorId="0">
+    <comment ref="B5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Jonny:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+We possibly need to think about some sort of 'game object' editor that includes lights, physics primitives, etc.  Otherwise it's just a case of pushing it through max.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B13" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Jonny:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Do we need shaders to be compiled into models?  Think about pros and cons.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B18" authorId="0">
       <text>
         <r>
           <rPr>
@@ -48,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="29">
   <si>
     <t>Task</t>
   </si>
@@ -77,26 +125,71 @@
     <t>Error handling strategy in Model Compiler - possibly use xsd?</t>
   </si>
   <si>
-    <t>Basic physics support - rigid body collisions</t>
-  </si>
-  <si>
     <t>Model compiler refactoring - wait till we have two surface formats implemented</t>
   </si>
   <si>
     <t>Get 64-bit scene exporter working</t>
   </si>
   <si>
-    <t>Spot lights</t>
-  </si>
-  <si>
-    <t>Spot lights within model</t>
+    <t>Module</t>
+  </si>
+  <si>
+    <t>Model Viewer</t>
+  </si>
+  <si>
+    <t>Engine</t>
+  </si>
+  <si>
+    <t>Bounding volume occlusion</t>
+  </si>
+  <si>
+    <t>Point lights</t>
+  </si>
+  <si>
+    <t>Add input manager with keyboard and mouse</t>
+  </si>
+  <si>
+    <t>Point lights in model chain</t>
+  </si>
+  <si>
+    <t>Rorn Pool</t>
+  </si>
+  <si>
+    <t>Build basic app</t>
+  </si>
+  <si>
+    <t>Compiled shaders</t>
+  </si>
+  <si>
+    <t>Game initialisation (position of balls, etc)</t>
+  </si>
+  <si>
+    <t>Basics of a physics engine</t>
+  </si>
+  <si>
+    <t>Player can move the cue ball (when appropriate)</t>
+  </si>
+  <si>
+    <t>Player can move cue</t>
+  </si>
+  <si>
+    <t>Player can take a shot</t>
+  </si>
+  <si>
+    <t>Scene Exporter</t>
+  </si>
+  <si>
+    <t>Model Compiler</t>
+  </si>
+  <si>
+    <t>Maths</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,6 +218,19 @@
       <name val="Tahoma"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -146,9 +252,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -450,119 +557,247 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B13"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="A20" sqref="A20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="91.5703125" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="91.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="B2">
+      <c r="C3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B12" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12">
         <v>10</v>
       </c>
-      <c r="B5">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>5</v>
-      </c>
-      <c r="B9">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
-      <c r="B13">
+      <c r="B13" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15">
         <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>28</v>
+      </c>
+      <c r="B19" t="s">
+        <v>3</v>
+      </c>
+      <c r="C19">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>13</v>
+      </c>
+      <c r="B20" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" t="s">
+        <v>5</v>
+      </c>
+      <c r="C21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>26</v>
+      </c>
+      <c r="B22" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Keyboard device capture is working.
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -560,7 +560,7 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -588,7 +588,7 @@
         <v>16</v>
       </c>
       <c r="C2" s="2">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Added mouse device to input manager. Implemented mouse controls in model viewer.
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -19,7 +19,31 @@
     <author>Jonny</author>
   </authors>
   <commentList>
-    <comment ref="B5" authorId="0">
+    <comment ref="B2" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Jonny:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+The camera inadvertantly rolls around :-(</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -43,7 +67,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B13" authorId="0">
+    <comment ref="B12" authorId="0">
       <text>
         <r>
           <rPr>
@@ -67,7 +91,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B18" authorId="0">
+    <comment ref="B17" authorId="0">
       <text>
         <r>
           <rPr>
@@ -96,7 +120,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="28">
   <si>
     <t>Task</t>
   </si>
@@ -144,9 +168,6 @@
   </si>
   <si>
     <t>Point lights</t>
-  </si>
-  <si>
-    <t>Add input manager with keyboard and mouse</t>
   </si>
   <si>
     <t>Point lights in model chain</t>
@@ -252,10 +273,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -557,10 +577,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -581,25 +601,25 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="2">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
         <v>6</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="C3">
-        <v>3</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -607,10 +627,10 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C4">
-        <v>21</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -618,7 +638,7 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C5">
         <v>7</v>
@@ -626,51 +646,51 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="C6">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C7">
-        <v>3</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
         <v>21</v>
       </c>
       <c r="C8">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
         <v>22</v>
       </c>
       <c r="C9">
-        <v>21</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s">
         <v>23</v>
@@ -681,46 +701,46 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B11" t="s">
         <v>24</v>
       </c>
       <c r="C11">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B12" t="s">
+        <v>19</v>
+      </c>
+      <c r="C12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>25</v>
       </c>
-      <c r="C12">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13">
-        <v>5</v>
+      <c r="B14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14">
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B15" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C15">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -728,18 +748,18 @@
         <v>26</v>
       </c>
       <c r="B16" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C16">
-        <v>4</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B17" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C17">
         <v>21</v>
@@ -750,21 +770,21 @@
         <v>27</v>
       </c>
       <c r="B18" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C18">
-        <v>21</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="B19" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C19">
-        <v>35</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -772,31 +792,20 @@
         <v>13</v>
       </c>
       <c r="B20" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C20">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="B21" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C21">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>26</v>
-      </c>
-      <c r="B22" t="s">
-        <v>10</v>
-      </c>
-      <c r="C22">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed free camera issue by regenerating matrix from euler angles each time.
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -19,31 +19,7 @@
     <author>Jonny</author>
   </authors>
   <commentList>
-    <comment ref="B2" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Jonny:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-The camera inadvertantly rolls around :-(</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B5" authorId="0">
+    <comment ref="B3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -67,7 +43,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B13" authorId="0">
+    <comment ref="B11" authorId="0">
       <text>
         <r>
           <rPr>
@@ -91,7 +67,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B18" authorId="0">
+    <comment ref="B17" authorId="0">
       <text>
         <r>
           <rPr>
@@ -120,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="27">
   <si>
     <t>Task</t>
   </si>
@@ -140,9 +116,6 @@
     <t>Add full screen support</t>
   </si>
   <si>
-    <t>Add camera controls to model viewer</t>
-  </si>
-  <si>
     <t>Revise, understand and document the view and projection matrix builds</t>
   </si>
   <si>
@@ -156,9 +129,6 @@
   </si>
   <si>
     <t>Module</t>
-  </si>
-  <si>
-    <t>Model Viewer</t>
   </si>
   <si>
     <t>Engine</t>
@@ -580,10 +550,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -594,7 +564,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -605,109 +575,109 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="C3">
-        <v>14</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C4">
-        <v>21</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B5" t="s">
         <v>16</v>
       </c>
       <c r="C5">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6">
         <v>14</v>
-      </c>
-      <c r="C6">
-        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C7">
-        <v>3</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
         <v>20</v>
       </c>
       <c r="C8">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
         <v>21</v>
       </c>
       <c r="C9">
-        <v>21</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s">
         <v>22</v>
       </c>
       <c r="C10">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
         <v>17</v>
-      </c>
-      <c r="B11" t="s">
-        <v>23</v>
       </c>
       <c r="C11">
         <v>5</v>
@@ -715,54 +685,54 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C12">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13">
-        <v>5</v>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14">
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B15" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C15">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B16" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C16">
-        <v>4</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B17" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C17">
         <v>21</v>
@@ -770,56 +740,45 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B18" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C18">
-        <v>21</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="B19" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C19">
-        <v>35</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B20" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C20">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="B21" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C21">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>25</v>
-      </c>
-      <c r="B22" t="s">
-        <v>10</v>
-      </c>
-      <c r="C22">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed camera bug.  Free camera now seems to do what I want it to!
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -19,7 +19,7 @@
     <author>Jonny</author>
   </authors>
   <commentList>
-    <comment ref="B5" authorId="0">
+    <comment ref="B4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -43,7 +43,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B13" authorId="0">
+    <comment ref="B12" authorId="0">
       <text>
         <r>
           <rPr>
@@ -67,7 +67,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B19" authorId="0">
+    <comment ref="B18" authorId="0">
       <text>
         <r>
           <rPr>
@@ -96,7 +96,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="28">
   <si>
     <t>Task</t>
   </si>
@@ -180,9 +180,6 @@
   </si>
   <si>
     <t>Invesitgate specular issue</t>
-  </si>
-  <si>
-    <t>Investigate camera issues</t>
   </si>
 </sst>
 </file>
@@ -557,10 +554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -592,14 +589,14 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" s="2">
-        <v>3</v>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3">
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -607,10 +604,10 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C4">
-        <v>21</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -618,7 +615,7 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C5">
         <v>7</v>
@@ -626,13 +623,13 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C6">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -640,32 +637,32 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C7">
-        <v>3</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C8">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C9">
-        <v>21</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -673,7 +670,7 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C10">
         <v>5</v>
@@ -684,21 +681,21 @@
         <v>15</v>
       </c>
       <c r="B11" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C11">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="C12">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -706,21 +703,21 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="C13">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" t="s">
-        <v>26</v>
-      </c>
-      <c r="C14">
         <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15">
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -728,21 +725,21 @@
         <v>23</v>
       </c>
       <c r="B16" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C16">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B17" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C17">
-        <v>4</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -750,7 +747,7 @@
         <v>24</v>
       </c>
       <c r="B18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C18">
         <v>21</v>
@@ -758,24 +755,24 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B19" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C19">
-        <v>21</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="B20" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C20">
-        <v>35</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -783,31 +780,20 @@
         <v>11</v>
       </c>
       <c r="B21" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C21">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="B22" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C22">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23" t="s">
-        <v>9</v>
-      </c>
-      <c r="C23">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated point lighting task.
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -19,31 +19,7 @@
     <author>Jonny</author>
   </authors>
   <commentList>
-    <comment ref="B4" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Jonny:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-We possibly need to think about some sort of 'game object' editor that includes lights, physics primitives, etc.  Otherwise it's just a case of pushing it through max.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B12" authorId="0">
+    <comment ref="B10" authorId="0">
       <text>
         <r>
           <rPr>
@@ -67,7 +43,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B18" authorId="0">
+    <comment ref="B16" authorId="0">
       <text>
         <r>
           <rPr>
@@ -96,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
   <si>
     <t>Task</t>
   </si>
@@ -137,12 +113,6 @@
     <t>Bounding volume occlusion</t>
   </si>
   <si>
-    <t>Point lights</t>
-  </si>
-  <si>
-    <t>Point lights in model chain</t>
-  </si>
-  <si>
     <t>Rorn Pool</t>
   </si>
   <si>
@@ -179,7 +149,7 @@
     <t>On-screen debug text</t>
   </si>
   <si>
-    <t>Invesitgate specular issue</t>
+    <t>Point lights - specular lighting</t>
   </si>
 </sst>
 </file>
@@ -249,10 +219,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -554,10 +523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -578,13 +547,13 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="2">
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2">
         <v>5</v>
       </c>
     </row>
@@ -593,84 +562,84 @@
         <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3">
-        <v>21</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
         <v>14</v>
       </c>
       <c r="C4">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C5">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C6">
-        <v>3</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
         <v>18</v>
       </c>
       <c r="C7">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
         <v>19</v>
       </c>
       <c r="C8">
-        <v>21</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
         <v>20</v>
       </c>
       <c r="C9">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
         <v>15</v>
-      </c>
-      <c r="B10" t="s">
-        <v>21</v>
       </c>
       <c r="C10">
         <v>5</v>
@@ -678,122 +647,100 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C11">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12">
-        <v>5</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="C13">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>21</v>
+      </c>
+      <c r="B14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14">
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B15" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="C15">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C16">
-        <v>4</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C17">
-        <v>21</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18">
         <v>7</v>
-      </c>
-      <c r="C18">
-        <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="B19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19">
         <v>3</v>
-      </c>
-      <c r="C19">
-        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="B20" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C20">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>11</v>
-      </c>
-      <c r="B21" t="s">
-        <v>5</v>
-      </c>
-      <c r="C21">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>23</v>
-      </c>
-      <c r="B22" t="s">
-        <v>9</v>
-      </c>
-      <c r="C22">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Standard distance units are now mm.
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -19,7 +19,7 @@
     <author>Jonny</author>
   </authors>
   <commentList>
-    <comment ref="B10" authorId="0">
+    <comment ref="B9" authorId="0">
       <text>
         <r>
           <rPr>
@@ -43,7 +43,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B16" authorId="0">
+    <comment ref="B15" authorId="0">
       <text>
         <r>
           <rPr>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
   <si>
     <t>Task</t>
   </si>
@@ -147,9 +147,6 @@
   </si>
   <si>
     <t>On-screen debug text</t>
-  </si>
-  <si>
-    <t>Point lights - specular lighting</t>
   </si>
 </sst>
 </file>
@@ -523,10 +520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -551,21 +548,21 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="C2">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C3">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -573,32 +570,32 @@
         <v>13</v>
       </c>
       <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4">
         <v>14</v>
-      </c>
-      <c r="C4">
-        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C5">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C6">
-        <v>21</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -606,7 +603,7 @@
         <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C7">
         <v>5</v>
@@ -617,21 +614,21 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C8">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="C9">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -639,21 +636,21 @@
         <v>11</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="C10">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11">
         <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12">
+        <v>14</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -661,21 +658,21 @@
         <v>21</v>
       </c>
       <c r="B13" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C13">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="B14" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14">
         <v>21</v>
-      </c>
-      <c r="B14" t="s">
-        <v>4</v>
-      </c>
-      <c r="C14">
-        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -683,7 +680,7 @@
         <v>22</v>
       </c>
       <c r="B15" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C15">
         <v>21</v>
@@ -691,24 +688,24 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B16" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C16">
-        <v>21</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="B17" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C17">
-        <v>35</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -716,31 +713,20 @@
         <v>11</v>
       </c>
       <c r="B18" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C18">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="B19" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C19">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" t="s">
-        <v>9</v>
-      </c>
-      <c r="C20">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Started to add support for export, compile and view.
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -19,7 +19,7 @@
     <author>Jonny</author>
   </authors>
   <commentList>
-    <comment ref="B9" authorId="0">
+    <comment ref="B12" authorId="0">
       <text>
         <r>
           <rPr>
@@ -43,7 +43,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B15" authorId="0">
+    <comment ref="B16" authorId="0">
       <text>
         <r>
           <rPr>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
   <si>
     <t>Task</t>
   </si>
@@ -147,6 +147,9 @@
   </si>
   <si>
     <t>On-screen debug text</t>
+  </si>
+  <si>
+    <t>FSAA</t>
   </si>
 </sst>
 </file>
@@ -216,9 +219,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -520,10 +524,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -545,35 +549,35 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="C2">
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="C3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="2">
         <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4">
-        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -581,10 +585,10 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C5">
-        <v>21</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -592,10 +596,10 @@
         <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C6">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -603,29 +607,29 @@
         <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C7">
-        <v>5</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B8" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C8">
-        <v>10</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="C9">
         <v>5</v>
@@ -633,45 +637,45 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C10">
-        <v>21</v>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="C12">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="C13">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14">
         <v>21</v>
       </c>
     </row>
@@ -680,7 +684,7 @@
         <v>22</v>
       </c>
       <c r="B15" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C15">
         <v>21</v>
@@ -688,24 +692,24 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B16" t="s">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="C16">
-        <v>35</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>11</v>
+        <v>23</v>
       </c>
       <c r="B17" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C17">
-        <v>7</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -713,20 +717,31 @@
         <v>11</v>
       </c>
       <c r="B18" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C18">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>21</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B20" t="s">
         <v>9</v>
       </c>
-      <c r="C19">
+      <c r="C20">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Made transition from Max->Viewer seamless.
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -19,7 +19,7 @@
     <author>Jonny</author>
   </authors>
   <commentList>
-    <comment ref="B12" authorId="0">
+    <comment ref="B10" authorId="0">
       <text>
         <r>
           <rPr>
@@ -43,7 +43,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B16" authorId="0">
+    <comment ref="B14" authorId="0">
       <text>
         <r>
           <rPr>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
   <si>
     <t>Task</t>
   </si>
@@ -80,13 +80,7 @@
     <t>Estimate</t>
   </si>
   <si>
-    <t>Make exporter a GUP.  Build UI &amp; hook data into the max files</t>
-  </si>
-  <si>
     <t>Complete the Rorn Maths library</t>
-  </si>
-  <si>
-    <t>Make the path from Max-&gt;Model Viewer seamless</t>
   </si>
   <si>
     <t>Add full screen support</t>
@@ -524,10 +518,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="A2" sqref="A2:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -538,7 +532,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -548,35 +542,35 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="A2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="2">
         <v>2</v>
-      </c>
-      <c r="C2">
-        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="C3">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C4" s="2">
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4">
         <v>2</v>
       </c>
     </row>
@@ -585,32 +579,32 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C5">
-        <v>4</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B7" t="s">
         <v>16</v>
       </c>
       <c r="C7">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -621,26 +615,26 @@
         <v>17</v>
       </c>
       <c r="C8">
-        <v>21</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B9" t="s">
         <v>18</v>
       </c>
       <c r="C9">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
         <v>13</v>
-      </c>
-      <c r="B10" t="s">
-        <v>19</v>
       </c>
       <c r="C10">
         <v>5</v>
@@ -648,100 +642,78 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C11">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12">
-        <v>5</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B13" t="s">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="C13">
         <v>21</v>
       </c>
     </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C14">
+        <v>21</v>
+      </c>
+    </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C15">
-        <v>21</v>
+        <v>35</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="B16" t="s">
+        <v>4</v>
+      </c>
+      <c r="C16">
         <v>7</v>
-      </c>
-      <c r="C16">
-        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="B17" t="s">
         <v>3</v>
       </c>
       <c r="C17">
-        <v>35</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C18">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>11</v>
-      </c>
-      <c r="B19" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>21</v>
-      </c>
-      <c r="B20" t="s">
-        <v>9</v>
-      </c>
-      <c r="C20">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added error handling on model load failure.
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -19,7 +19,7 @@
     <author>Jonny</author>
   </authors>
   <commentList>
-    <comment ref="B10" authorId="0">
+    <comment ref="B11" authorId="0">
       <text>
         <r>
           <rPr>
@@ -104,9 +104,6 @@
     <t>Engine</t>
   </si>
   <si>
-    <t>Bounding volume occlusion</t>
-  </si>
-  <si>
     <t>Rorn Pool</t>
   </si>
   <si>
@@ -144,6 +141,9 @@
   </si>
   <si>
     <t>FSAA</t>
+  </si>
+  <si>
+    <t>Bounding sphere occlusion</t>
   </si>
 </sst>
 </file>
@@ -521,7 +521,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD3"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -542,14 +542,14 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="2">
-        <v>2</v>
+      <c r="B2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2">
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -557,62 +557,62 @@
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="C3">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4">
+      <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
         <v>11</v>
       </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
       <c r="C5">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C6">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C7">
-        <v>5</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C8">
         <v>5</v>
@@ -620,24 +620,24 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C9">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="C10">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -645,15 +645,15 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="C11">
-        <v>21</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B13" t="s">
         <v>6</v>
@@ -664,7 +664,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B14" t="s">
         <v>5</v>
@@ -675,7 +675,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B15" t="s">
         <v>2</v>
@@ -708,7 +708,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B18" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Added FontBuilder to toolchain and updated on-screen debug text estimate.
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -521,7 +521,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -549,7 +549,7 @@
         <v>21</v>
       </c>
       <c r="C2">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Updated debug Font. Added font manager and new blit material. Added ability to add (1) debug text to the frame.
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -19,7 +19,7 @@
     <author>Jonny</author>
   </authors>
   <commentList>
-    <comment ref="B11" authorId="0">
+    <comment ref="B12" authorId="0">
       <text>
         <r>
           <rPr>
@@ -43,7 +43,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B14" authorId="0">
+    <comment ref="B15" authorId="0">
       <text>
         <r>
           <rPr>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
   <si>
     <t>Task</t>
   </si>
@@ -137,13 +137,16 @@
     <t>Maths</t>
   </si>
   <si>
-    <t>On-screen debug text</t>
-  </si>
-  <si>
     <t>FSAA</t>
   </si>
   <si>
     <t>Bounding sphere occlusion</t>
+  </si>
+  <si>
+    <t>Finish off debug rendering (text at least)</t>
+  </si>
+  <si>
+    <t>Engine refactoring (assume it is to be demoed</t>
   </si>
 </sst>
 </file>
@@ -518,10 +521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A2" sqref="A2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -542,14 +545,14 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2">
-        <v>14</v>
+      <c r="B2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" s="2">
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -564,24 +567,24 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="2">
-        <v>2</v>
+      <c r="C4">
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5">
+      <c r="A5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="2">
         <v>2</v>
       </c>
     </row>
@@ -590,32 +593,32 @@
         <v>10</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C6">
-        <v>14</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7">
         <v>14</v>
-      </c>
-      <c r="C7">
-        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C8">
-        <v>5</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -623,7 +626,7 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C9">
         <v>5</v>
@@ -634,32 +637,32 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C10">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>9</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B12" t="s">
         <v>12</v>
       </c>
-      <c r="C11">
+      <c r="C12">
         <v>5</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" t="s">
-        <v>6</v>
-      </c>
-      <c r="C13">
-        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -667,7 +670,7 @@
         <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C14">
         <v>21</v>
@@ -675,24 +678,24 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B15" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C15">
-        <v>35</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>9</v>
+        <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C16">
-        <v>7</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -700,20 +703,31 @@
         <v>9</v>
       </c>
       <c r="B17" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C17">
-        <v>3</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B18" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>18</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B19" t="s">
         <v>7</v>
       </c>
-      <c r="C18">
+      <c r="C19">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
1st major refactor pass complete.
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -19,7 +19,7 @@
     <author>Jonny</author>
   </authors>
   <commentList>
-    <comment ref="B12" authorId="0">
+    <comment ref="B10" authorId="0">
       <text>
         <r>
           <rPr>
@@ -43,7 +43,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B15" authorId="0">
+    <comment ref="B13" authorId="0">
       <text>
         <r>
           <rPr>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="23">
   <si>
     <t>Task</t>
   </si>
@@ -141,12 +141,6 @@
   </si>
   <si>
     <t>Bounding sphere occlusion</t>
-  </si>
-  <si>
-    <t>Finish off debug rendering (text at least)</t>
-  </si>
-  <si>
-    <t>Engine refactoring (assume it is to be demoed</t>
   </si>
 </sst>
 </file>
@@ -521,10 +515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C2"/>
+      <selection activeCell="A3" activeCellId="1" sqref="A2:XFD2 A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -545,58 +539,58 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="A2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="2">
-        <v>28</v>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2">
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3">
-        <v>4</v>
+      <c r="B3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="2">
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="C4">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" s="2">
-        <v>2</v>
+      <c r="A5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5">
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -604,21 +598,21 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C7">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C8">
-        <v>21</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -626,108 +620,86 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C9">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C10">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11">
-        <v>10</v>
-      </c>
-    </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C12">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>19</v>
+      </c>
+      <c r="B13" t="s">
         <v>5</v>
+      </c>
+      <c r="C13">
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C14">
-        <v>21</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>19</v>
+        <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C15">
-        <v>21</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="B16" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C16">
-        <v>35</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="B17" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C17">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>9</v>
-      </c>
-      <c r="B18" t="s">
-        <v>3</v>
-      </c>
-      <c r="C18">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>7</v>
-      </c>
-      <c r="C19">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Refactored RornMaths, Engine & ModelViewer so that it no longer references Vector3.
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -19,7 +19,7 @@
     <author>Jonny</author>
   </authors>
   <commentList>
-    <comment ref="B13" authorId="0">
+    <comment ref="B12" authorId="0">
       <text>
         <r>
           <rPr>
@@ -43,7 +43,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B16" authorId="0">
+    <comment ref="B15" authorId="0">
       <text>
         <r>
           <rPr>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
   <si>
     <t>Task</t>
   </si>
@@ -137,13 +137,10 @@
     <t>Bounding sphere occlusion</t>
   </si>
   <si>
-    <t>Complete Renderer refactoring</t>
-  </si>
-  <si>
-    <t>Deprecate Vector3.  Replace it with position, direction and unit direction</t>
-  </si>
-  <si>
     <t>Refactor index based unique container.  Think about using size_t rather than unsinged int.</t>
+  </si>
+  <si>
+    <t>Move to pre-compiled shaders</t>
   </si>
 </sst>
 </file>
@@ -518,10 +515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -549,7 +546,7 @@
         <v>21</v>
       </c>
       <c r="C2" s="2">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -557,42 +554,42 @@
         <v>8</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C3" s="2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="2">
+      <c r="C6">
         <v>2</v>
       </c>
     </row>
@@ -601,32 +598,32 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C7">
-        <v>2</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C8">
-        <v>14</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C9">
-        <v>35</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -634,7 +631,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C10">
         <v>5</v>
@@ -645,32 +642,32 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C11">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B12" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="C12">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C13">
         <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14" t="s">
+        <v>6</v>
+      </c>
+      <c r="C14">
+        <v>21</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -678,7 +675,7 @@
         <v>17</v>
       </c>
       <c r="B15" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C15">
         <v>21</v>
@@ -686,24 +683,24 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B16" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C16">
-        <v>21</v>
+        <v>35</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C17">
-        <v>35</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -711,20 +708,9 @@
         <v>8</v>
       </c>
       <c r="B18" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C18">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>8</v>
-      </c>
-      <c r="B19" t="s">
-        <v>3</v>
-      </c>
-      <c r="C19">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added support for multisampling.  It should work once its full screen!
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -19,7 +19,7 @@
     <author>Jonny</author>
   </authors>
   <commentList>
-    <comment ref="B12" authorId="0">
+    <comment ref="B10" authorId="0">
       <text>
         <r>
           <rPr>
@@ -43,7 +43,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B15" authorId="0">
+    <comment ref="B13" authorId="0">
       <text>
         <r>
           <rPr>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
   <si>
     <t>Task</t>
   </si>
@@ -131,16 +131,10 @@
     <t>Maths</t>
   </si>
   <si>
-    <t>FSAA</t>
-  </si>
-  <si>
     <t>Bounding sphere occlusion</t>
   </si>
   <si>
-    <t>Move to pre-compiled shaders</t>
-  </si>
-  <si>
-    <t>Refactor index based unique container?  Think about using size_t rather than unsinged int.</t>
+    <t>FSAA - requires full screen app</t>
   </si>
 </sst>
 </file>
@@ -515,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -543,54 +537,54 @@
         <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C2" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C3" s="2">
-        <v>5</v>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="C4">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="2">
-        <v>2</v>
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5">
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C6">
-        <v>2</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -598,21 +592,21 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C7">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B8" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C8">
-        <v>35</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -620,97 +614,75 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C9">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="C10">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C11">
-        <v>10</v>
-      </c>
-    </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="C12">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" t="s">
         <v>5</v>
+      </c>
+      <c r="C13">
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C14">
-        <v>21</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C15">
-        <v>21</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C16">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17" t="s">
-        <v>4</v>
-      </c>
-      <c r="C17">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18" t="s">
-        <v>3</v>
-      </c>
-      <c r="C18">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added new physics project and BaizeOfGlory project.  The the games begin.
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -19,7 +19,7 @@
     <author>Jonny</author>
   </authors>
   <commentList>
-    <comment ref="B10" authorId="0">
+    <comment ref="B9" authorId="0">
       <text>
         <r>
           <rPr>
@@ -43,7 +43,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B13" authorId="0">
+    <comment ref="B12" authorId="0">
       <text>
         <r>
           <rPr>
@@ -72,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
   <si>
     <t>Task</t>
   </si>
@@ -102,9 +102,6 @@
   </si>
   <si>
     <t>Rorn Pool</t>
-  </si>
-  <si>
-    <t>Build basic app</t>
   </si>
   <si>
     <t>Compiled shaders</t>
@@ -509,7 +506,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C16"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:XFD2"/>
@@ -533,14 +530,14 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" s="2">
-        <v>4</v>
+      <c r="A2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2">
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -548,43 +545,43 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C3">
+      <c r="C4" s="2">
         <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4">
-        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="C5">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B6" t="s">
         <v>13</v>
       </c>
       <c r="C6">
-        <v>35</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -606,37 +603,37 @@
         <v>15</v>
       </c>
       <c r="C8">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>16</v>
       </c>
-      <c r="C9">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C10">
-        <v>5</v>
+      <c r="B11" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11">
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C12">
         <v>21</v>
@@ -647,21 +644,21 @@
         <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C13">
-        <v>21</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C14">
-        <v>35</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -669,20 +666,9 @@
         <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C15">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16">
         <v>3</v>
       </c>
     </row>

</xml_diff>